<commit_message>
Nuevas validaciones A01-00006, A01-00007
</commit_message>
<xml_diff>
--- a/Analisis/validaciones/val_interfaces.xlsx
+++ b/Analisis/validaciones/val_interfaces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78ec6eafe1d282b6/Felipe/Projects/CMF/finReport/Analisis/validaciones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53A0F8DC-C297-4BCA-83E5-75A838A528AC}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="11_F25DC773A252ABDACC104864C11848EE5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D0FF94C-6E18-4CE9-9E6D-45645C41017D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,28 @@
     <sheet name="cartera_operaciones" sheetId="1" r:id="rId1"/>
     <sheet name="cuadro_operaciones" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>Campo a validar</t>
   </si>
@@ -207,6 +218,13 @@
 interno.tipo_deudor_rel</t>
   </si>
   <si>
+    <t>cod_tipo_obligacion</t>
+  </si>
+  <si>
+    <t>Verficia que la codificacion que se envia en la interfaz, exista en la tabla de relacion 
+interno.tabla_banco_126_rel</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Los reportantes pueden enviar la codificacion que solicita la CMF o enviar su codificacion interna, en caso de enviar codificacion interna, estos deben relacionar esta codificacion con la oficial de la CMF.
 Tabla principal: </t>
@@ -218,7 +236,7 @@
         <color theme="1"/>
         <rFont val="SimSun"/>
       </rPr>
-      <t>interno.tipo_deudor</t>
+      <t>interno.tabla_banco_126</t>
     </r>
     <r>
       <rPr>
@@ -236,6 +254,123 @@
         <color theme="1"/>
         <rFont val="SimSun"/>
       </rPr>
+      <t xml:space="preserve">interno.tabla_banco_126_rel 
+Como se mantiene:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t xml:space="preserve">Dentro de los directorios principales en AIRFLOW, existe una carpeta con nombre "mantenedores", ubicar el excel con nombre "tabla_banco_126.xlsx" y mantener la codificacion interna en la hoja "tabla_banco_126_rel", en la columna A debe ir la codificacion interna y en la columna B debe ir la codificacion oficial de la CMF.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t xml:space="preserve">Tips:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>- no borrar la relacion por default que esta en el excel
+- manejar los datos como tipo texto</t>
+    </r>
+  </si>
+  <si>
+    <t>cod_operacion</t>
+  </si>
+  <si>
+    <t>proceso.val_interfaz_B01</t>
+  </si>
+  <si>
+    <t>Verifica que las operaciones que se envian en la interfaz cuadro_operaciones, existan en la interfaz cartera_operaciones</t>
+  </si>
+  <si>
+    <t>Esto es problema de calidad de datos, netamente se debe solucionar en los extractores de la interfaz de cuadro_operaciones</t>
+  </si>
+  <si>
+    <t>Tipo validacion</t>
+  </si>
+  <si>
+    <t>Calidad de datos</t>
+  </si>
+  <si>
+    <t>logica</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>A01-00001</t>
+  </si>
+  <si>
+    <t>A01-00002</t>
+  </si>
+  <si>
+    <t>A01-00003</t>
+  </si>
+  <si>
+    <t>A01-00004</t>
+  </si>
+  <si>
+    <t>B01-00001</t>
+  </si>
+  <si>
+    <t>A01-00005</t>
+  </si>
+  <si>
+    <t>Esto es problema de calidad de datos, netamente se debe solucionar en los extractores de la interfaz de cartera_operaciones</t>
+  </si>
+  <si>
+    <t>Verifica que el campo cod_operacion exista en la interfaz cuadro_operaciones</t>
+  </si>
+  <si>
+    <t>ELIMINADA</t>
+  </si>
+  <si>
+    <t>ESTATUS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Los reportantes pueden enviar la codificacion que solicita la CMF o enviar su codificacion interna, en caso de enviar codificacion interna, estos deben relacionar esta codificacion con la oficial de la CMF.
+Tabla principal: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>interno.tipo_deudor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t xml:space="preserve">
+Tabla de relacion: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="SimSun"/>
+      </rPr>
       <t xml:space="preserve">interno.tipo_deudor_rel 
 Como se mantiene:
 </t>
@@ -243,7 +378,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color theme="0"/>
         <rFont val="SimSun"/>
       </rPr>
       <t xml:space="preserve">Dentro de los directorios principales en AIRFLOW, existe una carpeta con nombre "mantenedores", ubicar el excel con nombre "tipo_deudor.xlsx" y mantener la codificacion interna en la hoja "tipo_deudor_rel", en la columna A debe ir la codificacion interna y en la columna B debe ir la codificacion oficial de la CMF.
@@ -253,7 +388,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color theme="0"/>
         <rFont val="SimSun"/>
       </rPr>
       <t xml:space="preserve">Tips:
@@ -262,7 +397,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color theme="0"/>
         <rFont val="SimSun"/>
       </rPr>
       <t>- no borrar la relacion por default que esta en el excel
@@ -270,129 +405,26 @@
     </r>
   </si>
   <si>
-    <t>cod_tipo_obligacion</t>
-  </si>
-  <si>
-    <t>Verficia que la codificacion que se envia en la interfaz, exista en la tabla de relacion 
-interno.tabla_banco_126_rel</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Los reportantes pueden enviar la codificacion que solicita la CMF o enviar su codificacion interna, en caso de enviar codificacion interna, estos deben relacionar esta codificacion con la oficial de la CMF.
-Tabla principal: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t>interno.tabla_banco_126</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t xml:space="preserve">
-Tabla de relacion: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t xml:space="preserve">interno.tabla_banco_126_rel 
-Como se mantiene:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t xml:space="preserve">Dentro de los directorios principales en AIRFLOW, existe una carpeta con nombre "mantenedores", ubicar el excel con nombre "tabla_banco_126.xlsx" y mantener la codificacion interna en la hoja "tabla_banco_126_rel", en la columna A debe ir la codificacion interna y en la columna B debe ir la codificacion oficial de la CMF.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t xml:space="preserve">Tips:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="SimSun"/>
-      </rPr>
-      <t>- no borrar la relacion por default que esta en el excel
-- manejar los datos como tipo texto</t>
-    </r>
-  </si>
-  <si>
-    <t>cod_operacion</t>
-  </si>
-  <si>
-    <t>proceso.val_interfaz_B01</t>
-  </si>
-  <si>
-    <t>Verifica que las operaciones que se envian en la interfaz cuadro_operaciones, existan en la interfaz cartera_operaciones</t>
-  </si>
-  <si>
-    <t>Esto es problema de calidad de datos, netamente se debe solucionar en los extractores de la interfaz de cuadro_operaciones</t>
-  </si>
-  <si>
-    <t>Tipo validacion</t>
-  </si>
-  <si>
-    <t>Calidad de datos</t>
-  </si>
-  <si>
-    <t>logica</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>A01-00001</t>
-  </si>
-  <si>
-    <t>A01-00002</t>
-  </si>
-  <si>
-    <t>A01-00003</t>
-  </si>
-  <si>
-    <t>A01-00004</t>
-  </si>
-  <si>
-    <t>B01-00001</t>
-  </si>
-  <si>
-    <t>A01-00005</t>
-  </si>
-  <si>
-    <t>Esto es problema de calidad de datos, netamente se debe solucionar en los extractores de la interfaz de cartera_operaciones</t>
-  </si>
-  <si>
-    <t>Verifica que el campo cod_operacion exista en la interfaz cuadro_operaciones</t>
+    <t>A01-00006</t>
+  </si>
+  <si>
+    <t>Valida que la operacion este infoprmada solo una ves en la interfaz cartera_operaciones</t>
+  </si>
+  <si>
+    <t>A01-00007</t>
+  </si>
+  <si>
+    <t>fecha_otorgamiento</t>
+  </si>
+  <si>
+    <t>Valida que la fecha de otorgamiento sea menor o igual a la fecha de otorgamiento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,13 +443,30 @@
       <color theme="1"/>
       <name val="SimSun"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="SimSun"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="SimSun"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -432,10 +481,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -453,6 +506,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -718,10 +775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -733,9 +790,9 @@
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -744,7 +801,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -752,10 +809,13 @@
       <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="187.2" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="187.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -764,7 +824,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
@@ -773,9 +833,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="187.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="187.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -784,7 +844,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>7</v>
@@ -793,64 +853,107 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="187.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:7" ht="187.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="187.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="187.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -862,7 +965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C88A765-7EE8-4E01-AFBB-A48C7343D2A6}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -877,7 +980,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -886,7 +989,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -897,22 +1000,22 @@
     </row>
     <row r="2" spans="1:6" ht="29.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>